<commit_message>
new file:   e-commerce-JS-Project-iti/.vscode/settings.json 	modified:   e-commerce-JS-Project-iti/footer.css 	new file:   e-commerce-JS-Project-iti/index.html 	modified:   e-commerce-JS-Project-iti/javaScript project sheet.xlsx
</commit_message>
<xml_diff>
--- a/e-commerce-JS-Project-iti/javaScript project sheet.xlsx
+++ b/e-commerce-JS-Project-iti/javaScript project sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Files\ITI\Materials\Coding\JavaScript\final-project\js project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Files\ITI\Materials\Coding\JavaScript\final-project\js project\e-commerce-JS-Project-iti\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,9 +77,6 @@
     <t>customer dashboard (CSS)</t>
   </si>
   <si>
-    <t>admin dashboard(Edit product)</t>
-  </si>
-  <si>
     <t>customer dashboard (Add to shopping cart - checkout page</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>customer dashboard (search - see previous orders)</t>
+  </si>
+  <si>
+    <t>admin dashboard(Edit product - orders page)</t>
   </si>
 </sst>
 </file>
@@ -338,10 +338,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -661,7 +661,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -682,7 +682,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -704,11 +704,11 @@
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
@@ -750,15 +750,15 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -790,7 +790,7 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -798,7 +798,7 @@
     <row r="18" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11"/>
       <c r="C18" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>

</xml_diff>